<commit_message>
- update to v12.09
</commit_message>
<xml_diff>
--- a/output/spreadsheets/12.04/towers.xlsx
+++ b/output/spreadsheets/12.04/towers.xlsx
@@ -984,8 +984,7 @@
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>Analyzes the enemy within 7.00 range, allowing allies to attack the unit optimally (costs 5 energy) for 10.00 seconds. Target loses Spell Immunity and takes +8.00 spell damage per hit.
-Damage cooldown of 0.75 second.</t>
+          <t>Analyzes the enemy within 7.00 range, allowing allies to attack the unit optimally (costs 3 energy) for 10.00 seconds. Target takes +10.00 spell damage per hit.</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr"/>
@@ -1610,7 +1609,7 @@
       <c r="AG9" t="inlineStr">
         <is>
           <t>Archive will periodically perform a system-wide check that will restore nearby allies to their rightful stature. 
-Restores 24.00+8.00% shields every 8 seconds (on average) to 10.00 allies within 8.00 range.</t>
+Restores 24.00+8.00% shields every 8 seconds (on average) to 8.00 allies within 8.00 range.</t>
         </is>
       </c>
       <c r="AH9" t="inlineStr"/>
@@ -1985,7 +1984,7 @@
       <c r="AG12" t="inlineStr">
         <is>
           <t>Matriarchs strengthen ally shields within 8.00 range.
-Each grants +25.00% shields (max +150.00%).</t>
+Each grants +20.00% shields (max +120.00%).</t>
         </is>
       </c>
       <c r="AH12" t="inlineStr"/>
@@ -3799,7 +3798,7 @@
         <v/>
       </c>
       <c r="O27" t="n">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="P27" t="n">
         <v>16</v>
@@ -4575,7 +4574,7 @@
         <v>1</v>
       </c>
       <c r="Z33" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AA33">
         <f>T33/D33</f>
@@ -4601,7 +4600,7 @@
       </c>
       <c r="AG33" t="inlineStr">
         <is>
-          <t>An advanced quark generator emits a temporal resonance field that reverts damage to allies within 5 range. Up to 50 damage reverted per energy.</t>
+          <t>An advanced quark generator emits a temporal resonance field that reverts damage to allies within 6 range. Up to 100 damage reverted per energy.</t>
         </is>
       </c>
       <c r="AH33" t="inlineStr"/>
@@ -5920,7 +5919,7 @@
         <v>0</v>
       </c>
       <c r="R44" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="S44" t="n">
         <v>1</v>
@@ -6049,7 +6048,7 @@
         <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="S45" t="n">
         <v>1</v>
@@ -7222,7 +7221,7 @@
       </c>
       <c r="AG54" t="inlineStr">
         <is>
-          <t>Infatuates enemy send (not zergling) within 12.00 range for 8.00s. Attacks from infatuated units instead heal targets HP for 40.00% of attempted damage.
+          <t>Infatuates enemy send (not zergling) within 12.00 range for 8.00s. Attacks from infatuated units instead heal targets HP for 40.00% of attempted damage and restore 1.00 energy.
 Costs 45.00% hp.</t>
         </is>
       </c>
@@ -7472,7 +7471,7 @@
       </c>
       <c r="AG56" t="inlineStr">
         <is>
-          <t>Purges an enemy unit within 10.00 range removing Spell Immunity and dealing 300.00 damage. Costs 7 energy.</t>
+          <t>Purges an enemy unit within 10.00 range removing Spell Immunity and dealing 300.00 damage. Costs 5 energy.</t>
         </is>
       </c>
       <c r="AH56" t="inlineStr"/>
@@ -8283,7 +8282,7 @@
         <v>0</v>
       </c>
       <c r="R63" t="n">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="S63" t="n">
         <v>1</v>
@@ -8334,7 +8333,7 @@
       </c>
       <c r="AG63" t="inlineStr">
         <is>
-          <t>Each attack binds a Celestian to this Theos. Celestians so bound are released after 20.00s and have no collision.</t>
+          <t>Each attack spawns 1.00 Blessed Celestians that heal for an additional 3.00% life and ignore collisions. Every second attack spawns 1 additional Blessed Celestian. Limited to 130.00 alive at once per player.</t>
         </is>
       </c>
       <c r="AH63" t="inlineStr"/>
@@ -9328,7 +9327,7 @@
       <c r="AG71" t="inlineStr">
         <is>
           <t>Mudman covers attackers in mud slowing movement by 40.00% for 7.00 seconds. Max 5.00 stacks.
-On death applied applies a stack to enemies within 4.00 range, and refreshes duration of all existing stacks.</t>
+On death applies a stack to enemies within 4.00 range, and refreshes duration of all existing stacks.</t>
         </is>
       </c>
       <c r="AH71" t="inlineStr"/>
@@ -14755,7 +14754,8 @@
       </c>
       <c r="AG115" t="inlineStr">
         <is>
-          <t>At start of wave, grants allies within 2.00 range 30.00% chance to stun attackers for 2 seconds. 1.00 seconds cooldown after stunning an enemy.</t>
+          <t>At start of wave, grants allies within 2.00 range 30.00% chance to stun attackers for 2 seconds and reduce incoming damage by 20.00 + 50.00%.
+1.00 second cooldown after stunning an enemy.</t>
         </is>
       </c>
       <c r="AH115" t="inlineStr"/>
@@ -15003,7 +15003,7 @@
       </c>
       <c r="AG117" t="inlineStr">
         <is>
-          <t>Heals 6.00 allies within 7.00 range for 35.00 + 1.95% HP every 2.50 seconds (on average).</t>
+          <t>Heals 6.00 allies within 7.00 range for 35.00 + 1.95% HP every 2.00 seconds (on average).</t>
         </is>
       </c>
       <c r="AH117" t="inlineStr"/>
@@ -15376,7 +15376,7 @@
       <c r="AG120" t="inlineStr">
         <is>
           <t>The Dark Mage can entangle the mind of an ally within 5.00 range, increasing its attack speed by 30.00% for 20.00 seconds.
-Nightmare's gain +1 attacks for Counter-Attacks .
+Nightmare's gain +1 attacks for Counter-Attacks.
 Doppelganger gains +2 extra damage per attack with Fatality.
 Costs 10 energy.</t>
         </is>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="AH122" t="inlineStr">
         <is>
-          <t>Releases a fetid miasma on death that forms a dark swamp inflicting -1.00% hp/s on enemies caught within 2.00 range (max -4.00% hp/s). Additionally slows movement speed by 15.00% (max 60.00%). 
+          <t>Releases a fetid miasma on death that forms a dark swamp inflicting --1.00% hp/s on enemies caught within 2.00 range (max -4.00% hp/s). Additionally slows movement speed by 15.00% (max 60.00%). 
 Swamp lasts 5.00 seconds.</t>
         </is>
       </c>
@@ -15883,7 +15883,7 @@
       </c>
       <c r="AG124" t="inlineStr">
         <is>
-          <t>The unit's attacks slow the target's movement speed by 10.00% and attack speed by 7.00% for 4.00 seconds (max 6.00 stack; 2.00 per crawler).</t>
+          <t>The unit's attacks slow the target's movement speed by 15.00% and attack speed by 11.00% for 4.00 seconds (max 4.00 stack; 2.00 per crawler).</t>
         </is>
       </c>
       <c r="AH124" t="inlineStr"/>
@@ -18281,7 +18281,7 @@
       <c r="AH143" t="inlineStr">
         <is>
           <t>When triggered, attacks are 400.00% faster for 2.00 seconds and blind victims for 1.00 second.
-Additionally buffs 2.00 allies within 3.00 range. Their attacks are 100.00% faster for 2.00 seconds and blind victims for 1.00 second.
+Additionally buffs 2.00 allies within 4.00 range. Their attacks are 100.00% faster for 2.00 seconds and blind victims for 1.00 second.
 All stacks of Feed are lost when this ability ends.</t>
         </is>
       </c>
@@ -19388,10 +19388,10 @@
         <v>5</v>
       </c>
       <c r="P152" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="Q152" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="R152" t="n">
         <v>0.4</v>
@@ -19982,7 +19982,7 @@
       <c r="AI156" t="inlineStr">
         <is>
           <t>Grants composer 3 resolve mastery stacks.
-Each resolve stack grants 6.00% lifesteal from attacks.</t>
+Each resolve stack grants 5.00% lifesteal from attacks.</t>
         </is>
       </c>
     </row>
@@ -20371,7 +20371,7 @@
       <c r="AI159" t="inlineStr">
         <is>
           <t>Grants composer 3 resolve mastery stacks.
-Each resolve stack grants 6.00% lifesteal from attacks.</t>
+Each resolve stack grants 5.00% lifesteal from attacks.</t>
         </is>
       </c>
     </row>
@@ -20623,7 +20623,7 @@
       <c r="AG161" t="inlineStr">
         <is>
           <t>Grants composer 2 resolve mastery stack.
-Each resolve stack grants 6.00% lifesteal from attacks.</t>
+Each resolve stack grants 5.00% lifesteal from attacks.</t>
         </is>
       </c>
       <c r="AH161" t="inlineStr"/>
@@ -20753,7 +20753,7 @@
       <c r="AH162" t="inlineStr">
         <is>
           <t>Grants composer 4 resolve mastery stacks.
-Each resolve stack grants 6.00% lifesteal from attacks.</t>
+Each resolve stack grants 5.00% lifesteal from attacks.</t>
         </is>
       </c>
       <c r="AI162" t="inlineStr"/>
@@ -20885,7 +20885,7 @@
       <c r="AH163" t="inlineStr">
         <is>
           <t>Grants composer 3 resolve mastery stacks.
-Each resolve stack grants 6.00% lifesteal from attacks.</t>
+Each resolve stack grants 5.00% lifesteal from attacks.</t>
         </is>
       </c>
       <c r="AI163" t="inlineStr"/>
@@ -21873,7 +21873,7 @@
       </c>
       <c r="AG171" t="inlineStr">
         <is>
-          <t>Astralblade attacks cleave foes within a cone. 2.00 range, 90.00 degrees arc</t>
+          <t>Astralblade attacks cleave foes within a cone. 1.50 range, 90.00 degrees arc</t>
         </is>
       </c>
       <c r="AH171" t="inlineStr"/>
@@ -21997,7 +21997,7 @@
       </c>
       <c r="AG172" t="inlineStr">
         <is>
-          <t>Astralblade attacks cleave foes within a cone. 2.00 range, 100.00 degrees arc. Every 3rd attack stuns enemies for 1.5 seconds.</t>
+          <t>Astralblade attacks cleave foes within a cone. 1.50 range, 100.00 degrees arc. Every 3rd attack stuns enemies for 1.5 seconds.</t>
         </is>
       </c>
       <c r="AH172" t="inlineStr"/>
@@ -23012,7 +23012,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>405</v>
+        <v>330</v>
       </c>
       <c r="E181" t="n">
         <v>420</v>
@@ -23733,7 +23733,7 @@
       </c>
       <c r="AG186" t="inlineStr">
         <is>
-          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Ji'nara restores shields by 100.00% of consumed vitals.</t>
+          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Ji'nara restores shields by 50.00% of consumed vitals (150.00% if summon or tier 1 Tal'darim consumed).</t>
         </is>
       </c>
       <c r="AH186" t="inlineStr"/>
@@ -23857,7 +23857,7 @@
       </c>
       <c r="AG187" t="inlineStr">
         <is>
-          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Alarak restores shields by 125.00% of consumed vitals.</t>
+          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Alarak restores shields by 85.00% of consumed vitals (200.00% if summon or tier 1 Tal'darim consumed).</t>
         </is>
       </c>
       <c r="AH187" t="inlineStr"/>
@@ -23981,7 +23981,7 @@
       </c>
       <c r="AG188" t="inlineStr">
         <is>
-          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Alarak restores shields by 125.00% of consumed vitals.
+          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Alarak restores shields by 85.00% of consumed vitals (200.00% if summon or tier 1 Tal'darim consumed).
 On each sacrifice, Alarak releases a Destruction Wave towards attacker, damaging all units in its path for 20.00% of sacrificed unit's vitals.</t>
         </is>
       </c>
@@ -24106,7 +24106,7 @@
       </c>
       <c r="AG189" t="inlineStr">
         <is>
-          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Alarak restores shields by 125.00% of consumed vitals.
+          <t>Prevents fatal blow by consuming a summon or a tier 1 Tal'darim unit within 10.10 radius. If no such units exist, instead consumes all shields of an ally (ally must have more than 750.00 current shields). By doing so, Alarak restores shields by 85.00% of consumed vitals (200.00% if summon or tier 1 Tal'darim consumed).
 On each sacrifice, Alarak stuns nearby foes based on sacrificed vitals (1 sec per 2000.00 vitals drained).</t>
         </is>
       </c>

</xml_diff>